<commit_message>
DY - modify excel template file
</commit_message>
<xml_diff>
--- a/modules/export/src/main/resources/templates/template_Simam_import_Regimen.xlsx
+++ b/modules/export/src/main/resources/templates/template_Simam_import_Regimen.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CdUniS</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>${program_code}</t>
+  </si>
+  <si>
+    <t>${movDescID}</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -525,6 +528,9 @@
       </c>
     </row>
     <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>

</xml_diff>